<commit_message>
RHA 2020 et + : CSARR et CCAM ok
</commit_message>
<xml_diff>
--- a/formats/excel/Formats RHA 20.xlsx
+++ b/formats/excel/Formats RHA 20.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10404"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumepressiat/Documents/Developpements/Github/formats_pmeasyr/formats/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8685134A-14D0-9948-8519-54F1BE26AAE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F02419C-32D5-C742-891F-DF5955EF2AF4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="16340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -757,10 +757,10 @@
   <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomRight" activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2363,7 +2363,7 @@
       </c>
       <c r="F67" s="1">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G67" t="s">
         <v>9</v>
@@ -2374,7 +2374,7 @@
         <v>125</v>
       </c>
       <c r="D68">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" t="s">

</xml_diff>